<commit_message>
Fix of the following issues : 1. Updating invoice records in database
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1356,7 +1356,7 @@
       </c>
       <c r="F2" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2021-05-19 </t>
+          <t xml:space="preserve">2021-06-06 </t>
         </is>
       </c>
       <c r="H2" s="1" t="n"/>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>INV202105191307</t>
+          <t>INV202106061149</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1439,7 +1439,11 @@
       <c r="H8" s="69" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="22" t="inlineStr"/>
+      <c r="A9" s="22" t="inlineStr">
+        <is>
+          <t>Anurag Deo</t>
+        </is>
+      </c>
       <c r="B9" s="64" t="n"/>
       <c r="C9" s="64" t="n"/>
       <c r="D9" s="64" t="n"/>
@@ -1459,7 +1463,11 @@
       <c r="F10" s="24" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="22" t="inlineStr"/>
+      <c r="A11" s="22" t="inlineStr">
+        <is>
+          <t>Bangalore South</t>
+        </is>
+      </c>
       <c r="B11" s="64" t="n"/>
       <c r="C11" s="64" t="n"/>
       <c r="D11" s="64" t="n"/>
@@ -1480,7 +1488,11 @@
       <c r="H12" s="4" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="22" t="inlineStr"/>
+      <c r="A13" s="22" t="inlineStr">
+        <is>
+          <t>990019344</t>
+        </is>
+      </c>
       <c r="B13" s="64" t="n"/>
       <c r="C13" s="64" t="n"/>
       <c r="D13" s="64" t="n"/>
@@ -1528,13 +1540,21 @@
           <t>Admin</t>
         </is>
       </c>
-      <c r="B16" s="13" t="inlineStr"/>
+      <c r="B16" s="13" t="inlineStr">
+        <is>
+          <t>Anurag Deo</t>
+        </is>
+      </c>
       <c r="C16" s="19" t="inlineStr">
         <is>
           <t>Not Available</t>
         </is>
       </c>
-      <c r="D16" s="19" t="inlineStr"/>
+      <c r="D16" s="19" t="inlineStr">
+        <is>
+          <t>990019344</t>
+        </is>
+      </c>
       <c r="E16" s="64" t="n"/>
       <c r="F16" s="24" t="n"/>
       <c r="H16" s="5" t="n"/>
@@ -1582,12 +1602,36 @@
       <c r="H18" s="69" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="inlineStr"/>
-      <c r="B19" s="12" t="inlineStr"/>
-      <c r="C19" s="7" t="inlineStr"/>
-      <c r="D19" s="14" t="inlineStr"/>
-      <c r="E19" s="7" t="inlineStr"/>
-      <c r="F19" s="32" t="inlineStr"/>
+      <c r="A19" s="31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B19" s="12" t="inlineStr">
+        <is>
+          <t>Test Book 9</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D19" s="14" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E19" s="7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F19" s="32" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
       <c r="H19" s="5" t="n"/>
     </row>
     <row r="20">
@@ -1687,7 +1731,7 @@
       <c r="E29" s="61" t="n"/>
       <c r="F29" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>200</t>
         </is>
       </c>
       <c r="H29" s="69" t="n"/>

</xml_diff>

<commit_message>
Fix of the following issue - 1. Print function does not work in sales window 2. Code refactoring for namin conventions in sales module 3. Exit button exceeds screen width in sales screen .
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1356,7 +1356,7 @@
       </c>
       <c r="F2" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2021-06-06 </t>
+          <t xml:space="preserve">2021-06-10 </t>
         </is>
       </c>
       <c r="H2" s="1" t="n"/>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>INV202106061149</t>
+          <t>INV202106101423</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1441,7 +1441,7 @@
     <row r="9">
       <c r="A9" s="22" t="inlineStr">
         <is>
-          <t>Anurag Deo</t>
+          <t>Sant Anurag Deo</t>
         </is>
       </c>
       <c r="B9" s="64" t="n"/>
@@ -1465,7 +1465,7 @@
     <row r="11">
       <c r="A11" s="22" t="inlineStr">
         <is>
-          <t>Bangalore South</t>
+          <t>Bangalore East,Karnataka</t>
         </is>
       </c>
       <c r="B11" s="64" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="13">
       <c r="A13" s="22" t="inlineStr">
         <is>
-          <t>990019344</t>
+          <t>9900019861</t>
         </is>
       </c>
       <c r="B13" s="64" t="n"/>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="B16" s="13" t="inlineStr">
         <is>
-          <t>Anurag Deo</t>
+          <t>Sant Anurag Deo</t>
         </is>
       </c>
       <c r="C16" s="19" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>990019344</t>
+          <t>9900019861</t>
         </is>
       </c>
       <c r="E16" s="64" t="n"/>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="B19" s="12" t="inlineStr">
         <is>
-          <t>Test Book 9</t>
+          <t>Introduction To Vihangam Yoga</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
@@ -1619,17 +1619,17 @@
       </c>
       <c r="D19" s="14" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E19" s="7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F19" s="32" t="inlineStr">
+        <is>
           <t>100</t>
-        </is>
-      </c>
-      <c r="E19" s="7" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F19" s="32" t="inlineStr">
-        <is>
-          <t>200</t>
         </is>
       </c>
       <c r="H19" s="5" t="n"/>
@@ -1731,7 +1731,7 @@
       <c r="E29" s="61" t="n"/>
       <c r="F29" s="36" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>100</t>
         </is>
       </c>
       <c r="H29" s="69" t="n"/>

</xml_diff>

<commit_message>
Fix of the following issue - 1. Invoice id is not generated
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>INV202106101423</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1465,7 +1465,7 @@
     <row r="11">
       <c r="A11" s="22" t="inlineStr">
         <is>
-          <t>Bangalore East,Karnataka</t>
+          <t xml:space="preserve">Bangalore East </t>
         </is>
       </c>
       <c r="B11" s="64" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="13">
       <c r="A13" s="22" t="inlineStr">
         <is>
-          <t>9900019861</t>
+          <t>990019361</t>
         </is>
       </c>
       <c r="B13" s="64" t="n"/>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>9900019861</t>
+          <t>990019361</t>
         </is>
       </c>
       <c r="E16" s="64" t="n"/>

</xml_diff>

<commit_message>
Fix of following issues: 1. Reset Cart doesn't reset the cart. 2. All Main menu buttons remain enabled after reset Cart .
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1356,7 +1356,7 @@
       </c>
       <c r="F2" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2021-06-10 </t>
+          <t xml:space="preserve">2021-06-21 </t>
         </is>
       </c>
       <c r="H2" s="1" t="n"/>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1439,11 +1439,7 @@
       <c r="H8" s="69" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="22" t="inlineStr">
-        <is>
-          <t>Sant Anurag Deo</t>
-        </is>
-      </c>
+      <c r="A9" s="22" t="inlineStr"/>
       <c r="B9" s="64" t="n"/>
       <c r="C9" s="64" t="n"/>
       <c r="D9" s="64" t="n"/>
@@ -1463,11 +1459,7 @@
       <c r="F10" s="24" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bangalore East </t>
-        </is>
-      </c>
+      <c r="A11" s="22" t="inlineStr"/>
       <c r="B11" s="64" t="n"/>
       <c r="C11" s="64" t="n"/>
       <c r="D11" s="64" t="n"/>
@@ -1488,11 +1480,7 @@
       <c r="H12" s="4" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="22" t="inlineStr">
-        <is>
-          <t>990019361</t>
-        </is>
-      </c>
+      <c r="A13" s="22" t="inlineStr"/>
       <c r="B13" s="64" t="n"/>
       <c r="C13" s="64" t="n"/>
       <c r="D13" s="64" t="n"/>
@@ -1540,21 +1528,13 @@
           <t>Admin</t>
         </is>
       </c>
-      <c r="B16" s="13" t="inlineStr">
-        <is>
-          <t>Sant Anurag Deo</t>
-        </is>
-      </c>
+      <c r="B16" s="13" t="inlineStr"/>
       <c r="C16" s="19" t="inlineStr">
         <is>
           <t>Not Available</t>
         </is>
       </c>
-      <c r="D16" s="19" t="inlineStr">
-        <is>
-          <t>990019361</t>
-        </is>
-      </c>
+      <c r="D16" s="19" t="inlineStr"/>
       <c r="E16" s="64" t="n"/>
       <c r="F16" s="24" t="n"/>
       <c r="H16" s="5" t="n"/>

</xml_diff>

<commit_message>
Fix of the following issue: 1. Points earned is not credited to customer account
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1356,7 +1356,7 @@
       </c>
       <c r="F2" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2021-06-21 </t>
+          <t xml:space="preserve">2021-06-28 </t>
         </is>
       </c>
       <c r="H2" s="1" t="n"/>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1439,7 +1439,11 @@
       <c r="H8" s="69" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="22" t="inlineStr"/>
+      <c r="A9" s="22" t="inlineStr">
+        <is>
+          <t>Sant Anurag Deo</t>
+        </is>
+      </c>
       <c r="B9" s="64" t="n"/>
       <c r="C9" s="64" t="n"/>
       <c r="D9" s="64" t="n"/>
@@ -1459,7 +1463,11 @@
       <c r="F10" s="24" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="22" t="inlineStr"/>
+      <c r="A11" s="22" t="inlineStr">
+        <is>
+          <t>102, Whitestone veroso, Banglore 49</t>
+        </is>
+      </c>
       <c r="B11" s="64" t="n"/>
       <c r="C11" s="64" t="n"/>
       <c r="D11" s="64" t="n"/>
@@ -1480,7 +1488,11 @@
       <c r="H12" s="4" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="22" t="inlineStr"/>
+      <c r="A13" s="22" t="inlineStr">
+        <is>
+          <t>9900019362</t>
+        </is>
+      </c>
       <c r="B13" s="64" t="n"/>
       <c r="C13" s="64" t="n"/>
       <c r="D13" s="64" t="n"/>
@@ -1528,13 +1540,21 @@
           <t>Admin</t>
         </is>
       </c>
-      <c r="B16" s="13" t="inlineStr"/>
+      <c r="B16" s="13" t="inlineStr">
+        <is>
+          <t>Sant Anurag Deo</t>
+        </is>
+      </c>
       <c r="C16" s="19" t="inlineStr">
         <is>
           <t>Not Available</t>
         </is>
       </c>
-      <c r="D16" s="19" t="inlineStr"/>
+      <c r="D16" s="19" t="inlineStr">
+        <is>
+          <t>9900019362</t>
+        </is>
+      </c>
       <c r="E16" s="64" t="n"/>
       <c r="F16" s="24" t="n"/>
       <c r="H16" s="5" t="n"/>
@@ -1589,17 +1609,17 @@
       </c>
       <c r="B19" s="12" t="inlineStr">
         <is>
-          <t>Introduction To Vihangam Yoga</t>
+          <t>Test Book106</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D19" s="14" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">

</xml_diff>

<commit_message>
Fix of the following issue: 1. Current redeem points  earned is not shown in sales window for customer account
</commit_message>
<xml_diff>
--- a/Library_Stock/Invoices/Template/sales-invoice.xlsx
+++ b/Library_Stock/Invoices/Template/sales-invoice.xlsx
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F3" s="63" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H3" s="2" t="n"/>
@@ -1465,7 +1465,7 @@
     <row r="11">
       <c r="A11" s="22" t="inlineStr">
         <is>
-          <t>102, Whitestone veroso, Banglore 49</t>
+          <t>102, Whitestone Veroso, Bangalore 560049</t>
         </is>
       </c>
       <c r="B11" s="64" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="13">
       <c r="A13" s="22" t="inlineStr">
         <is>
-          <t>9900019362</t>
+          <t>9900019361</t>
         </is>
       </c>
       <c r="B13" s="64" t="n"/>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="D16" s="19" t="inlineStr">
         <is>
-          <t>9900019362</t>
+          <t>9900019361</t>
         </is>
       </c>
       <c r="E16" s="64" t="n"/>
@@ -1609,17 +1609,17 @@
       </c>
       <c r="B19" s="12" t="inlineStr">
         <is>
-          <t>Test Book106</t>
+          <t>Test Book73</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D19" s="14" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
@@ -1629,27 +1629,75 @@
       </c>
       <c r="F19" s="32" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>20</t>
         </is>
       </c>
       <c r="H19" s="5" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="33" t="inlineStr"/>
-      <c r="B20" s="20" t="inlineStr"/>
-      <c r="C20" s="8" t="inlineStr"/>
-      <c r="D20" s="15" t="inlineStr"/>
-      <c r="E20" s="8" t="inlineStr"/>
-      <c r="F20" s="34" t="inlineStr"/>
+      <c r="A20" s="33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B20" s="20" t="inlineStr">
+        <is>
+          <t>Test Book78</t>
+        </is>
+      </c>
+      <c r="C20" s="8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" s="15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F20" s="34" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
       <c r="H20" s="69" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="33" t="inlineStr"/>
-      <c r="B21" s="20" t="inlineStr"/>
-      <c r="C21" s="8" t="inlineStr"/>
-      <c r="D21" s="15" t="inlineStr"/>
-      <c r="E21" s="8" t="inlineStr"/>
-      <c r="F21" s="34" t="inlineStr"/>
+      <c r="A21" s="33" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B21" s="20" t="inlineStr">
+        <is>
+          <t>Test Book76</t>
+        </is>
+      </c>
+      <c r="C21" s="8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D21" s="15" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F21" s="34" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
       <c r="H21" s="69" t="n"/>
     </row>
     <row r="22">
@@ -1731,7 +1779,7 @@
       <c r="E29" s="61" t="n"/>
       <c r="F29" s="36" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>190</t>
         </is>
       </c>
       <c r="H29" s="69" t="n"/>

</xml_diff>